<commit_message>
Update Excel analysis with average per student
</commit_message>
<xml_diff>
--- a/student_performance.xlsx
+++ b/student_performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e1d9f429f2230465/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{07FCE0EA-24C7-42E1-A1A7-E05C46832F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FEA9F04-61C5-4731-8801-D7126AEF0094}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{07FCE0EA-24C7-42E1-A1A7-E05C46832F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A093C57-DBE8-4238-8F42-4601AE024B64}"/>
   <bookViews>
-    <workbookView xWindow="10370" yWindow="820" windowWidth="8660" windowHeight="8970" xr2:uid="{6C228E55-347D-4E57-A4EF-F25F76B8FCE0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6C228E55-347D-4E57-A4EF-F25F76B8FCE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
     <t>kriti</t>
   </si>
   <si>
-    <t>Average_Marks</t>
+    <t>Average_Per_Student</t>
   </si>
 </sst>
 </file>
@@ -167,6 +167,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.25775890487385511"/>
+          <c:y val="4.1230905652798348E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -203,8 +211,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.0358705161854749E-2"/>
-          <c:y val="0.19486111111111112"/>
+          <c:x val="7.8348109737596178E-2"/>
+          <c:y val="0.11785840151276872"/>
           <c:w val="0.89019685039370078"/>
           <c:h val="0.72088764946048411"/>
         </c:manualLayout>
@@ -457,7 +465,350 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN"/>
+              <a:t>Average Marks per Student</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15543866963870492"/>
+          <c:y val="0.25908758891228351"/>
+          <c:w val="0.79873795282156546"/>
+          <c:h val="0.57886379287205647"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A0D2-4481-84AB-8D7A13988E34}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="315264687"/>
+        <c:axId val="348177007"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="315264687"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="348177007"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="348177007"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="315264687"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1000,20 +1351,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>911225</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>175962</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>33421</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>489479</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1038,7 +1892,47 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>462359</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>166292</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1025260</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>132292</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFD897FC-D044-90F9-E711-2AC88A569887}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1340,8 +2234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774A072E-E5B7-44E3-9AB5-10CF34156206}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1349,7 +2243,7 @@
     <col min="1" max="1" width="17.26953125" customWidth="1"/>
     <col min="2" max="2" width="14.7265625" customWidth="1"/>
     <col min="3" max="3" width="12.90625" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" customWidth="1"/>
+    <col min="4" max="4" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1376,6 +2270,10 @@
       <c r="C2" s="1">
         <v>78</v>
       </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D7" si="0">AVERAGEIF(A:A, A2, C:C)</f>
+        <v>78</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -1387,6 +2285,10 @@
       <c r="C3" s="1">
         <v>85</v>
       </c>
+      <c r="D3">
+        <f>AVERAGEIF(A:A, A3, C:C)</f>
+        <v>85</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -1398,6 +2300,10 @@
       <c r="C4" s="1">
         <v>65</v>
       </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -1409,6 +2315,10 @@
       <c r="C5" s="1">
         <v>72</v>
       </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -1420,6 +2330,10 @@
       <c r="C6" s="1">
         <v>90</v>
       </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -1429,6 +2343,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="1">
+        <v>88</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
         <v>88</v>
       </c>
     </row>

</xml_diff>